<commit_message>
added circuit breaker to server in hw7a
</commit_message>
<xml_diff>
--- a/2a/2a.xlsx
+++ b/2a/2a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyujiang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyujiang/Desktop/6650/CS6650/2a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CE94A6-9883-E748-B059-2B789AF98D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1804F52-8B90-1743-95EB-02732013AD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{4FBD58C0-6BE1-EA4E-B5E4-52879B95F0CB}"/>
   </bookViews>
@@ -50,22 +50,7 @@
     <t>Time taken(ms)</t>
   </si>
   <si>
-    <t>Time taken to add elements to Vector (ms)</t>
-  </si>
-  <si>
-    <t>Time taken to add 100k elements to ArrayList (ms)</t>
-  </si>
-  <si>
     <t>Results from the collection 2 program</t>
-  </si>
-  <si>
-    <t>Time taken to add elements to HashMap (ms)</t>
-  </si>
-  <si>
-    <t>Time taken to add elements to ConcurrentHashMap (ms)</t>
-  </si>
-  <si>
-    <t>Time taken to add elements to HashTable (ms)</t>
   </si>
   <si>
     <t>Results from the multithreaded file writer program</t>
@@ -85,12 +70,27 @@
   <si>
     <t>Number of threads generated</t>
   </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>HashMap</t>
+  </si>
+  <si>
+    <t>HashTable</t>
+  </si>
+  <si>
+    <t>ConcurrentHashMap</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,11 +140,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF1F2328"/>
-      <name val="Var(--fontStack-monospace, ui-m"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF1F2328"/>
@@ -173,14 +168,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -319,7 +313,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$B$20,Sheet1!$B$21:$B$23)</c:f>
+              <c:f>(Sheet1!$B$19,Sheet1!$B$20:$B$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -340,7 +334,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$C$20,Sheet1!$C$21:$C$23)</c:f>
+              <c:f>(Sheet1!$C$19,Sheet1!$C$20:$C$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -410,7 +404,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$B$20,Sheet1!$B$21:$B$23)</c:f>
+              <c:f>(Sheet1!$B$19,Sheet1!$B$20:$B$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -431,7 +425,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$D$20,Sheet1!$D$21:$D$23)</c:f>
+              <c:f>(Sheet1!$D$19,Sheet1!$D$20:$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -501,7 +495,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$B$20,Sheet1!$B$21:$B$23)</c:f>
+              <c:f>(Sheet1!$B$19,Sheet1!$B$20:$B$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -522,7 +516,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$E$20,Sheet1!$E$21:$E$23)</c:f>
+              <c:f>(Sheet1!$E$19,Sheet1!$E$20:$E$22)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -893,7 +887,497 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Use a Single Thread to add 100K Elements</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$8:$A$9,Sheet1!$A$13:$A$15)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>ArrayList</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Vector</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HashMap</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HashTable</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ConcurrentHashMap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$B$8:$B$9,Sheet1!$B$13:$B$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F08F-6040-B70A-7418C83CF018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="247"/>
+        <c:axId val="1742848160"/>
+        <c:axId val="1742849888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1742848160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Different</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Data Strucutres</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1742849888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1742849888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time Taken to add elements</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1742848160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1449,6 +1933,555 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="221">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1461,7 +2494,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1482,6 +2515,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29B1AC1A-3EB6-0520-159A-972A16B1A935}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1807,13 +2876,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BAA8F34-7DF7-0543-B3A5-2D73315C1D3B}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="2"/>
@@ -1821,18 +2890,18 @@
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1847,7 +2916,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +2933,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1881,49 +2950,57 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
+      <c r="C12" s="2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="B14" s="2">
         <v>7</v>
@@ -1932,98 +3009,87 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E19" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>157</v>
+      </c>
+      <c r="C20" s="2">
+        <v>291</v>
+      </c>
+      <c r="D20" s="2">
+        <v>561</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2">
-        <v>14</v>
+      <c r="B21" s="2">
+        <v>122</v>
+      </c>
+      <c r="C21" s="2">
+        <v>155</v>
+      </c>
+      <c r="D21" s="2">
+        <v>306</v>
+      </c>
+      <c r="E21" s="2">
+        <v>468</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="3" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2000</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5000</v>
-      </c>
-      <c r="E20" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="2">
-        <v>157</v>
-      </c>
-      <c r="C21" s="2">
-        <v>291</v>
-      </c>
-      <c r="D21" s="2">
-        <v>561</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B22" s="2">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="C22" s="2">
-        <v>155</v>
+        <v>348</v>
       </c>
       <c r="D22" s="2">
-        <v>306</v>
+        <v>828</v>
       </c>
       <c r="E22" s="2">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="2">
-        <v>196</v>
-      </c>
-      <c r="C23" s="2">
-        <v>348</v>
-      </c>
-      <c r="D23" s="2">
-        <v>828</v>
-      </c>
-      <c r="E23" s="2">
         <v>1395</v>
       </c>
     </row>

</xml_diff>